<commit_message>
updated to 3d line chart
</commit_message>
<xml_diff>
--- a/data/sample.xlsx
+++ b/data/sample.xlsx
@@ -222,13 +222,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.45"/>
   </cols>
@@ -266,8 +266,44 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="3" t="n">
+        <v>6000</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>7505</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>7240</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>8520</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7542</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>6542</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8542</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>9545</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>